<commit_message>
default data file upload
</commit_message>
<xml_diff>
--- a/data/happy.xlsx
+++ b/data/happy.xlsx
@@ -434,9 +434,9 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -463,7 +463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -479,7 +479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -503,7 +503,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -511,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -519,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -528,7 +528,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -537,7 +537,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -558,15 +558,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -580,7 +580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -592,27 +592,13 @@
       </c>
       <c r="D2">
         <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D16" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D15" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>